<commit_message>
minor bug fixes, improved sorting
- reorder xlsx file by index (row 48 was at very bottom)
- fix bug caused by empty rows
- improve sorting (implement multi level sorting)
- minor code clean-up
- replot all
</commit_message>
<xml_diff>
--- a/Open_Science_Survey_BN_cln.xlsx
+++ b/Open_Science_Survey_BN_cln.xlsx
@@ -1103,6 +1103,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AC55" totalsRowShown="0">
   <autoFilter ref="A1:AC55"/>
+  <sortState ref="A2:AC55">
+    <sortCondition ref="A1:A55"/>
+  </sortState>
   <tableColumns count="29">
     <tableColumn id="1" name="ID" dataDxfId="28"/>
     <tableColumn id="6" name="Position:" dataDxfId="27"/>
@@ -1437,7 +1440,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O55" sqref="O55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5707,96 +5712,92 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>53</v>
+        <v>187</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>31</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>290</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="O49" s="1"/>
       <c r="P49" s="1" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="S49" s="1" t="s">
         <v>36</v>
       </c>
       <c r="T49" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="U49" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="V49" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="X49" s="1" t="s">
-        <v>291</v>
+        <v>247</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z49" s="1" t="s">
-        <v>292</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="Z49" s="1"/>
       <c r="AA49" s="1" t="s">
-        <v>293</v>
+        <v>132</v>
       </c>
       <c r="AB49" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="AC49" s="1" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>53</v>
@@ -5805,19 +5806,19 @@
         <v>30</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>31</v>
@@ -5829,49 +5830,49 @@
         <v>32</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>294</v>
+        <v>94</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="S50" s="1" t="s">
         <v>36</v>
       </c>
       <c r="T50" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="U50" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="V50" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X50" s="1" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="Z50" s="1" t="s">
-        <v>99</v>
+        <v>292</v>
       </c>
       <c r="AA50" s="1" t="s">
         <v>293</v>
@@ -5885,31 +5886,31 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>32</v>
@@ -5924,44 +5925,46 @@
         <v>32</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>117</v>
+        <v>294</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>209</v>
+        <v>103</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="R51" s="1" t="s">
         <v>48</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="T51" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="U51" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="W51" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="X51" s="1" t="s">
-        <v>297</v>
+        <v>247</v>
       </c>
       <c r="Y51" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z51" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="Z51" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="AA51" s="1" t="s">
-        <v>42</v>
+        <v>293</v>
       </c>
       <c r="AB51" s="1" t="s">
         <v>38</v>
@@ -5972,25 +5975,25 @@
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>32</v>
@@ -6002,69 +6005,67 @@
         <v>32</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>299</v>
+        <v>209</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="R52" s="1" t="s">
         <v>48</v>
       </c>
       <c r="S52" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="T52" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="U52" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="V52" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="W52" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="X52" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="Y52" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z52" s="1" t="s">
-        <v>301</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="Z52" s="1"/>
       <c r="AA52" s="1" t="s">
         <v>42</v>
       </c>
       <c r="AB52" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="AC52" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>30</v>
@@ -6076,67 +6077,67 @@
         <v>30</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R53" s="1" t="s">
         <v>48</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="T53" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="U53" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="V53" s="1" t="s">
         <v>38</v>
       </c>
       <c r="W53" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X53" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="Y53" s="1" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="Z53" s="1" t="s">
-        <v>195</v>
+        <v>301</v>
       </c>
       <c r="AA53" s="1" t="s">
         <v>42</v>
@@ -6145,72 +6146,72 @@
         <v>43</v>
       </c>
       <c r="AC53" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>31</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M54" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>38</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="T54" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U54" s="1" t="s">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c r="V54" s="1" t="s">
         <v>38</v>
@@ -6219,30 +6220,30 @@
         <v>38</v>
       </c>
       <c r="X54" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="Y54" s="1" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="Z54" s="1" t="s">
-        <v>308</v>
+        <v>195</v>
       </c>
       <c r="AA54" s="1" t="s">
         <v>42</v>
       </c>
       <c r="AB54" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="AC54" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>187</v>
+        <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>32</v>
@@ -6251,13 +6252,13 @@
         <v>32</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>32</v>
@@ -6269,57 +6270,61 @@
         <v>31</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="O55" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>305</v>
+      </c>
       <c r="P55" s="1" t="s">
-        <v>180</v>
+        <v>306</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>38</v>
       </c>
       <c r="R55" s="1" t="s">
-        <v>48</v>
+        <v>170</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U55" s="1" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="V55" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="X55" s="1" t="s">
-        <v>247</v>
+        <v>307</v>
       </c>
       <c r="Y55" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z55" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="Z55" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="AA55" s="1" t="s">
-        <v>132</v>
+        <v>42</v>
       </c>
       <c r="AB55" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC55" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="AC55" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>